<commit_message>
Updated requirements and cleaning
</commit_message>
<xml_diff>
--- a/output/cousybo01.xlsx
+++ b/output/cousybo01.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="81">
   <si>
     <t>Season</t>
   </si>
@@ -720,7 +720,7 @@
         <v>5.3</v>
       </c>
       <c r="O2">
-        <v>0.7559999999999999</v>
+        <v>0.756</v>
       </c>
       <c r="P2">
         <v>6.9</v>
@@ -814,7 +814,7 @@
         <v>0.7000000000000002</v>
       </c>
       <c r="O4">
-        <v>0.07700000000000007</v>
+        <v>0.07699999999999996</v>
       </c>
       <c r="P4">
         <v>0.5999999999999996</v>
@@ -870,7 +870,7 @@
         <v>7.7</v>
       </c>
       <c r="O5">
-        <v>0.8079999999999999</v>
+        <v>0.8080000000000001</v>
       </c>
       <c r="P5">
         <v>6.4</v>
@@ -970,7 +970,7 @@
         <v>6.999999999999999</v>
       </c>
       <c r="O7">
-        <v>0.1240000000000001</v>
+        <v>0.124</v>
       </c>
       <c r="P7">
         <v>-2.4</v>
@@ -1117,7 +1117,7 @@
         <v>1.399999999999999</v>
       </c>
       <c r="L10">
-        <v>0.03099999999999992</v>
+        <v>0.03100000000000003</v>
       </c>
       <c r="M10">
         <v>3.499999999999999</v>
@@ -1494,7 +1494,7 @@
         <v>7.8</v>
       </c>
       <c r="O17">
-        <v>0.8440000000000001</v>
+        <v>0.844</v>
       </c>
       <c r="P17">
         <v>6.8</v>
@@ -1594,7 +1594,7 @@
         <v>0.5000000000000009</v>
       </c>
       <c r="O19">
-        <v>0.07599999999999996</v>
+        <v>0.07600000000000007</v>
       </c>
       <c r="P19">
         <v>1.2</v>
@@ -1641,7 +1641,7 @@
         <v>19.8</v>
       </c>
       <c r="L20">
-        <v>0.3779999999999999</v>
+        <v>0.378</v>
       </c>
       <c r="M20">
         <v>5.7</v>
@@ -1741,7 +1741,7 @@
         <v>0.8999999999999986</v>
       </c>
       <c r="L22">
-        <v>-0.05399999999999994</v>
+        <v>-0.05399999999999999</v>
       </c>
       <c r="M22">
         <v>1.1</v>
@@ -2333,7 +2333,7 @@
         <v>8.800000000000001</v>
       </c>
       <c r="O33">
-        <v>0.7609999999999999</v>
+        <v>0.761</v>
       </c>
       <c r="P33">
         <v>4.3</v>
@@ -2374,7 +2374,7 @@
         <v>2.9</v>
       </c>
       <c r="O34">
-        <v>-0.01800000000000013</v>
+        <v>-0.01800000000000002</v>
       </c>
       <c r="P34">
         <v>-0.1000000000000005</v>
@@ -2521,7 +2521,7 @@
         <v>1.5</v>
       </c>
       <c r="L37">
-        <v>-0.03399999999999997</v>
+        <v>-0.03400000000000003</v>
       </c>
       <c r="M37">
         <v>0.4000000000000004</v>
@@ -2932,7 +2932,7 @@
         <v>6.3</v>
       </c>
       <c r="O55">
-        <v>0.8029999999999999</v>
+        <v>0.803</v>
       </c>
       <c r="P55">
         <v>5.2</v>
@@ -2985,7 +2985,7 @@
         <v>7.3</v>
       </c>
       <c r="O56">
-        <v>0.8009999999999999</v>
+        <v>0.801</v>
       </c>
       <c r="P56">
         <v>5</v>
@@ -3131,7 +3131,7 @@
         <v>6.2</v>
       </c>
       <c r="O60">
-        <v>0.8029999999999999</v>
+        <v>0.803</v>
       </c>
       <c r="P60">
         <v>5.2</v>
@@ -3181,7 +3181,7 @@
         <v>7.3</v>
       </c>
       <c r="O61">
-        <v>0.8009999999999999</v>
+        <v>0.801</v>
       </c>
       <c r="P61">
         <v>5</v>
@@ -3244,12 +3244,2423 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:T50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>69</v>
+      </c>
+      <c r="L2">
+        <v>0.352</v>
+      </c>
+      <c r="O2">
+        <v>0.756</v>
+      </c>
+      <c r="T2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>0.214</v>
+      </c>
+      <c r="O3">
+        <v>0.833</v>
+      </c>
+      <c r="T3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>-0.138</v>
+      </c>
+      <c r="O4">
+        <v>0.07699999999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5">
+        <v>66</v>
+      </c>
+      <c r="I5">
+        <v>2681</v>
+      </c>
+      <c r="J5">
+        <v>6.9</v>
+      </c>
+      <c r="K5">
+        <v>18.6</v>
+      </c>
+      <c r="L5">
+        <v>0.369</v>
+      </c>
+      <c r="M5">
+        <v>5.5</v>
+      </c>
+      <c r="N5">
+        <v>6.8</v>
+      </c>
+      <c r="O5">
+        <v>0.8080000000000001</v>
+      </c>
+      <c r="P5">
+        <v>5.7</v>
+      </c>
+      <c r="Q5">
+        <v>5.9</v>
+      </c>
+      <c r="R5">
+        <v>2.6</v>
+      </c>
+      <c r="S5">
+        <v>19.2</v>
+      </c>
+      <c r="T5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="I6">
+        <v>138</v>
+      </c>
+      <c r="J6">
+        <v>6.8</v>
+      </c>
+      <c r="K6">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>0.4</v>
+      </c>
+      <c r="M6">
+        <v>10.7</v>
+      </c>
+      <c r="N6">
+        <v>11.5</v>
+      </c>
+      <c r="O6">
+        <v>0.9320000000000001</v>
+      </c>
+      <c r="P6">
+        <v>3.1</v>
+      </c>
+      <c r="Q6">
+        <v>5</v>
+      </c>
+      <c r="R6">
+        <v>3.4</v>
+      </c>
+      <c r="S6">
+        <v>24.3</v>
+      </c>
+      <c r="T6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>-2543</v>
+      </c>
+      <c r="J7">
+        <v>-0.1000000000000005</v>
+      </c>
+      <c r="K7">
+        <v>-1.600000000000001</v>
+      </c>
+      <c r="L7">
+        <v>0.03100000000000003</v>
+      </c>
+      <c r="M7">
+        <v>5.199999999999999</v>
+      </c>
+      <c r="N7">
+        <v>4.7</v>
+      </c>
+      <c r="O7">
+        <v>0.124</v>
+      </c>
+      <c r="P7">
+        <v>-2.6</v>
+      </c>
+      <c r="Q7">
+        <v>-0.9000000000000004</v>
+      </c>
+      <c r="R7">
+        <v>0.7999999999999998</v>
+      </c>
+      <c r="S7">
+        <v>5.100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8">
+        <v>71</v>
+      </c>
+      <c r="I8">
+        <v>2945</v>
+      </c>
+      <c r="J8">
+        <v>5.7</v>
+      </c>
+      <c r="K8">
+        <v>16.1</v>
+      </c>
+      <c r="L8">
+        <v>0.352</v>
+      </c>
+      <c r="M8">
+        <v>5.9</v>
+      </c>
+      <c r="N8">
+        <v>7.2</v>
+      </c>
+      <c r="O8">
+        <v>0.8159999999999999</v>
+      </c>
+      <c r="P8">
+        <v>5.5</v>
+      </c>
+      <c r="Q8">
+        <v>6.7</v>
+      </c>
+      <c r="R8">
+        <v>2.8</v>
+      </c>
+      <c r="S8">
+        <v>17.2</v>
+      </c>
+      <c r="T8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="I9">
+        <v>270</v>
+      </c>
+      <c r="J9">
+        <v>6.1</v>
+      </c>
+      <c r="K9">
+        <v>16</v>
+      </c>
+      <c r="L9">
+        <v>0.383</v>
+      </c>
+      <c r="M9">
+        <v>8.1</v>
+      </c>
+      <c r="N9">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="O9">
+        <v>0.836</v>
+      </c>
+      <c r="P9">
+        <v>3.3</v>
+      </c>
+      <c r="Q9">
+        <v>4.9</v>
+      </c>
+      <c r="R9">
+        <v>2.8</v>
+      </c>
+      <c r="S9">
+        <v>20.4</v>
+      </c>
+      <c r="T9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>-2675</v>
+      </c>
+      <c r="J10">
+        <v>0.3999999999999995</v>
+      </c>
+      <c r="K10">
+        <v>-0.1000000000000014</v>
+      </c>
+      <c r="L10">
+        <v>0.03100000000000003</v>
+      </c>
+      <c r="M10">
+        <v>2.199999999999999</v>
+      </c>
+      <c r="N10">
+        <v>2.499999999999999</v>
+      </c>
+      <c r="O10">
+        <v>0.02000000000000002</v>
+      </c>
+      <c r="P10">
+        <v>-2.2</v>
+      </c>
+      <c r="Q10">
+        <v>-1.8</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>3.199999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11">
+        <v>72</v>
+      </c>
+      <c r="I11">
+        <v>2857</v>
+      </c>
+      <c r="J11">
+        <v>6.1</v>
+      </c>
+      <c r="K11">
+        <v>15.9</v>
+      </c>
+      <c r="L11">
+        <v>0.385</v>
+      </c>
+      <c r="M11">
+        <v>5.2</v>
+      </c>
+      <c r="N11">
+        <v>6.6</v>
+      </c>
+      <c r="O11">
+        <v>0.787</v>
+      </c>
+      <c r="P11">
+        <v>5</v>
+      </c>
+      <c r="Q11">
+        <v>6.5</v>
+      </c>
+      <c r="R11">
+        <v>2.5</v>
+      </c>
+      <c r="S11">
+        <v>17.4</v>
+      </c>
+      <c r="T11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>260</v>
+      </c>
+      <c r="J12">
+        <v>4.6</v>
+      </c>
+      <c r="K12">
+        <v>16.1</v>
+      </c>
+      <c r="L12">
+        <v>0.284</v>
+      </c>
+      <c r="M12">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="N12">
+        <v>10.4</v>
+      </c>
+      <c r="O12">
+        <v>0.8</v>
+      </c>
+      <c r="P12">
+        <v>4.4</v>
+      </c>
+      <c r="Q12">
+        <v>5.3</v>
+      </c>
+      <c r="R12">
+        <v>2.8</v>
+      </c>
+      <c r="S12">
+        <v>17.4</v>
+      </c>
+      <c r="T12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>-2597</v>
+      </c>
+      <c r="J13">
+        <v>-1.5</v>
+      </c>
+      <c r="K13">
+        <v>0.2000000000000011</v>
+      </c>
+      <c r="L13">
+        <v>-0.101</v>
+      </c>
+      <c r="M13">
+        <v>3.100000000000001</v>
+      </c>
+      <c r="N13">
+        <v>3.800000000000001</v>
+      </c>
+      <c r="O13">
+        <v>0.01300000000000001</v>
+      </c>
+      <c r="P13">
+        <v>-0.5999999999999996</v>
+      </c>
+      <c r="Q13">
+        <v>-1.2</v>
+      </c>
+      <c r="R13">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" t="s">
+        <v>66</v>
+      </c>
+      <c r="G14">
+        <v>71</v>
+      </c>
+      <c r="I14">
+        <v>2747</v>
+      </c>
+      <c r="J14">
+        <v>6.8</v>
+      </c>
+      <c r="K14">
+        <v>17.2</v>
+      </c>
+      <c r="L14">
+        <v>0.397</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>7.5</v>
+      </c>
+      <c r="O14">
+        <v>0.8070000000000001</v>
+      </c>
+      <c r="P14">
+        <v>5.6</v>
+      </c>
+      <c r="Q14">
+        <v>7.3</v>
+      </c>
+      <c r="R14">
+        <v>2.2</v>
+      </c>
+      <c r="S14">
+        <v>19.7</v>
+      </c>
+      <c r="T14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="I15">
+        <v>299</v>
+      </c>
+      <c r="J15">
+        <v>6.4</v>
+      </c>
+      <c r="K15">
+        <v>16.7</v>
+      </c>
+      <c r="L15">
+        <v>0.381</v>
+      </c>
+      <c r="M15">
+        <v>5.5</v>
+      </c>
+      <c r="N15">
+        <v>5.8</v>
+      </c>
+      <c r="O15">
+        <v>0.958</v>
+      </c>
+      <c r="P15">
+        <v>5.2</v>
+      </c>
+      <c r="Q15">
+        <v>7.8</v>
+      </c>
+      <c r="R15">
+        <v>3.1</v>
+      </c>
+      <c r="S15">
+        <v>18.3</v>
+      </c>
+      <c r="T15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>-2448</v>
+      </c>
+      <c r="J16">
+        <v>-0.3999999999999995</v>
+      </c>
+      <c r="K16">
+        <v>-0.5</v>
+      </c>
+      <c r="L16">
+        <v>-0.01600000000000001</v>
+      </c>
+      <c r="M16">
+        <v>-0.5</v>
+      </c>
+      <c r="N16">
+        <v>-1.7</v>
+      </c>
+      <c r="O16">
+        <v>0.1509999999999999</v>
+      </c>
+      <c r="P16">
+        <v>-0.3999999999999995</v>
+      </c>
+      <c r="Q16">
+        <v>0.5</v>
+      </c>
+      <c r="R16">
+        <v>0.8999999999999999</v>
+      </c>
+      <c r="S16">
+        <v>-1.399999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G17">
+        <v>72</v>
+      </c>
+      <c r="I17">
+        <v>2767</v>
+      </c>
+      <c r="J17">
+        <v>5.7</v>
+      </c>
+      <c r="K17">
+        <v>15.9</v>
+      </c>
+      <c r="L17">
+        <v>0.36</v>
+      </c>
+      <c r="M17">
+        <v>6.2</v>
+      </c>
+      <c r="N17">
+        <v>7.3</v>
+      </c>
+      <c r="O17">
+        <v>0.844</v>
+      </c>
+      <c r="P17">
+        <v>6.4</v>
+      </c>
+      <c r="Q17">
+        <v>8.4</v>
+      </c>
+      <c r="R17">
+        <v>2.7</v>
+      </c>
+      <c r="S17">
+        <v>17.6</v>
+      </c>
+      <c r="T17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" t="s">
+        <v>65</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18">
+        <v>3</v>
+      </c>
+      <c r="I18">
+        <v>124</v>
+      </c>
+      <c r="J18">
+        <v>8.1</v>
+      </c>
+      <c r="K18">
+        <v>16.3</v>
+      </c>
+      <c r="L18">
+        <v>0.5</v>
+      </c>
+      <c r="M18">
+        <v>6.7</v>
+      </c>
+      <c r="N18">
+        <v>7.3</v>
+      </c>
+      <c r="O18">
+        <v>0.92</v>
+      </c>
+      <c r="P18">
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <v>7.5</v>
+      </c>
+      <c r="R18">
+        <v>1.2</v>
+      </c>
+      <c r="S18">
+        <v>22.9</v>
+      </c>
+      <c r="T18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>-2643</v>
+      </c>
+      <c r="J19">
+        <v>2.399999999999999</v>
+      </c>
+      <c r="K19">
+        <v>0.4000000000000004</v>
+      </c>
+      <c r="L19">
+        <v>0.14</v>
+      </c>
+      <c r="M19">
+        <v>0.5</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0.07600000000000007</v>
+      </c>
+      <c r="P19">
+        <v>0.5999999999999996</v>
+      </c>
+      <c r="Q19">
+        <v>-0.9000000000000004</v>
+      </c>
+      <c r="R19">
+        <v>-1.5</v>
+      </c>
+      <c r="S19">
+        <v>5.299999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>65</v>
+      </c>
+      <c r="F20" t="s">
+        <v>66</v>
+      </c>
+      <c r="G20">
+        <v>64</v>
+      </c>
+      <c r="I20">
+        <v>2364</v>
+      </c>
+      <c r="J20">
+        <v>7.3</v>
+      </c>
+      <c r="K20">
+        <v>19.2</v>
+      </c>
+      <c r="L20">
+        <v>0.378</v>
+      </c>
+      <c r="M20">
+        <v>5.5</v>
+      </c>
+      <c r="N20">
+        <v>6.7</v>
+      </c>
+      <c r="O20">
+        <v>0.821</v>
+      </c>
+      <c r="P20">
+        <v>4.7</v>
+      </c>
+      <c r="Q20">
+        <v>7.3</v>
+      </c>
+      <c r="R20">
+        <v>2</v>
+      </c>
+      <c r="S20">
+        <v>20.1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>65</v>
+      </c>
+      <c r="F21" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21">
+        <v>10</v>
+      </c>
+      <c r="I21">
+        <v>440</v>
+      </c>
+      <c r="J21">
+        <v>5.5</v>
+      </c>
+      <c r="K21">
+        <v>16.9</v>
+      </c>
+      <c r="L21">
+        <v>0.324</v>
+      </c>
+      <c r="M21">
+        <v>5.6</v>
+      </c>
+      <c r="N21">
+        <v>7.4</v>
+      </c>
+      <c r="O21">
+        <v>0.747</v>
+      </c>
+      <c r="P21">
+        <v>5</v>
+      </c>
+      <c r="Q21">
+        <v>7.6</v>
+      </c>
+      <c r="R21">
+        <v>2.2</v>
+      </c>
+      <c r="S21">
+        <v>16.5</v>
+      </c>
+      <c r="T21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <v>-1924</v>
+      </c>
+      <c r="J22">
+        <v>-1.8</v>
+      </c>
+      <c r="K22">
+        <v>-2.300000000000001</v>
+      </c>
+      <c r="L22">
+        <v>-0.05399999999999999</v>
+      </c>
+      <c r="M22">
+        <v>0.09999999999999964</v>
+      </c>
+      <c r="N22">
+        <v>0.7000000000000002</v>
+      </c>
+      <c r="O22">
+        <v>-0.07399999999999995</v>
+      </c>
+      <c r="P22">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="Q22">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="R22">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="S22">
+        <v>-3.600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E23" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23">
+        <v>65</v>
+      </c>
+      <c r="I23">
+        <v>2222</v>
+      </c>
+      <c r="J23">
+        <v>7.2</v>
+      </c>
+      <c r="K23">
+        <v>20.4</v>
+      </c>
+      <c r="L23">
+        <v>0.353</v>
+      </c>
+      <c r="M23">
+        <v>4.5</v>
+      </c>
+      <c r="N23">
+        <v>5.3</v>
+      </c>
+      <c r="O23">
+        <v>0.85</v>
+      </c>
+      <c r="P23">
+        <v>5.2</v>
+      </c>
+      <c r="Q23">
+        <v>7.5</v>
+      </c>
+      <c r="R23">
+        <v>2.2</v>
+      </c>
+      <c r="S23">
+        <v>18.9</v>
+      </c>
+      <c r="T23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>457</v>
+      </c>
+      <c r="J24">
+        <v>5.3</v>
+      </c>
+      <c r="K24">
+        <v>15.4</v>
+      </c>
+      <c r="L24">
+        <v>0.342</v>
+      </c>
+      <c r="M24">
+        <v>5</v>
+      </c>
+      <c r="N24">
+        <v>5.9</v>
+      </c>
+      <c r="O24">
+        <v>0.853</v>
+      </c>
+      <c r="P24">
+        <v>5.6</v>
+      </c>
+      <c r="Q24">
+        <v>6.5</v>
+      </c>
+      <c r="R24">
+        <v>1.6</v>
+      </c>
+      <c r="S24">
+        <v>15.6</v>
+      </c>
+      <c r="T24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="I25">
+        <v>-1765</v>
+      </c>
+      <c r="J25">
+        <v>-1.9</v>
+      </c>
+      <c r="K25">
+        <v>-4.999999999999998</v>
+      </c>
+      <c r="L25">
+        <v>-0.01099999999999995</v>
+      </c>
+      <c r="M25">
+        <v>0.5</v>
+      </c>
+      <c r="N25">
+        <v>0.6000000000000005</v>
+      </c>
+      <c r="O25">
+        <v>0.003000000000000003</v>
+      </c>
+      <c r="P25">
+        <v>0.3999999999999995</v>
+      </c>
+      <c r="Q25">
+        <v>-1</v>
+      </c>
+      <c r="R25">
+        <v>-0.6000000000000001</v>
+      </c>
+      <c r="S25">
+        <v>-3.299999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" t="s">
+        <v>66</v>
+      </c>
+      <c r="G26">
+        <v>65</v>
+      </c>
+      <c r="I26">
+        <v>2403</v>
+      </c>
+      <c r="J26">
+        <v>7.3</v>
+      </c>
+      <c r="K26">
+        <v>18.9</v>
+      </c>
+      <c r="L26">
+        <v>0.384</v>
+      </c>
+      <c r="M26">
+        <v>4.9</v>
+      </c>
+      <c r="N26">
+        <v>5.8</v>
+      </c>
+      <c r="O26">
+        <v>0.855</v>
+      </c>
+      <c r="P26">
+        <v>5.4</v>
+      </c>
+      <c r="Q26">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="R26">
+        <v>2</v>
+      </c>
+      <c r="S26">
+        <v>19.4</v>
+      </c>
+      <c r="T26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>66</v>
+      </c>
+      <c r="G27">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>460</v>
+      </c>
+      <c r="J27">
+        <v>5.6</v>
+      </c>
+      <c r="K27">
+        <v>17.3</v>
+      </c>
+      <c r="L27">
+        <v>0.326</v>
+      </c>
+      <c r="M27">
+        <v>5.5</v>
+      </c>
+      <c r="N27">
+        <v>7.4</v>
+      </c>
+      <c r="O27">
+        <v>0.745</v>
+      </c>
+      <c r="P27">
+        <v>5.9</v>
+      </c>
+      <c r="Q27">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="R27">
+        <v>2.2</v>
+      </c>
+      <c r="S27">
+        <v>16.7</v>
+      </c>
+      <c r="T27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="I28">
+        <v>-1943</v>
+      </c>
+      <c r="J28">
+        <v>-1.7</v>
+      </c>
+      <c r="K28">
+        <v>-1.599999999999998</v>
+      </c>
+      <c r="L28">
+        <v>-0.058</v>
+      </c>
+      <c r="M28">
+        <v>0.5999999999999996</v>
+      </c>
+      <c r="N28">
+        <v>1.600000000000001</v>
+      </c>
+      <c r="O28">
+        <v>-0.11</v>
+      </c>
+      <c r="P28">
+        <v>0.5</v>
+      </c>
+      <c r="Q28">
+        <v>1</v>
+      </c>
+      <c r="R28">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="S28">
+        <v>-2.699999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F29" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29">
+        <v>75</v>
+      </c>
+      <c r="I29">
+        <v>2588</v>
+      </c>
+      <c r="J29">
+        <v>7.9</v>
+      </c>
+      <c r="K29">
+        <v>20.6</v>
+      </c>
+      <c r="L29">
+        <v>0.384</v>
+      </c>
+      <c r="M29">
+        <v>4.4</v>
+      </c>
+      <c r="N29">
+        <v>5.6</v>
+      </c>
+      <c r="O29">
+        <v>0.792</v>
+      </c>
+      <c r="P29">
+        <v>4.9</v>
+      </c>
+      <c r="Q29">
+        <v>9.9</v>
+      </c>
+      <c r="R29">
+        <v>2</v>
+      </c>
+      <c r="S29">
+        <v>20.2</v>
+      </c>
+      <c r="T29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>51</v>
+      </c>
+      <c r="D30" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>65</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30">
+        <v>13</v>
+      </c>
+      <c r="I30">
+        <v>468</v>
+      </c>
+      <c r="J30">
+        <v>6.2</v>
+      </c>
+      <c r="K30">
+        <v>20.2</v>
+      </c>
+      <c r="L30">
+        <v>0.305</v>
+      </c>
+      <c r="M30">
+        <v>3</v>
+      </c>
+      <c r="N30">
+        <v>3.9</v>
+      </c>
+      <c r="O30">
+        <v>0.765</v>
+      </c>
+      <c r="P30">
+        <v>3.7</v>
+      </c>
+      <c r="Q30">
+        <v>8.9</v>
+      </c>
+      <c r="R30">
+        <v>2.1</v>
+      </c>
+      <c r="S30">
+        <v>15.3</v>
+      </c>
+      <c r="T30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="I31">
+        <v>-2120</v>
+      </c>
+      <c r="J31">
+        <v>-1.7</v>
+      </c>
+      <c r="K31">
+        <v>-0.4000000000000021</v>
+      </c>
+      <c r="L31">
+        <v>-0.07900000000000001</v>
+      </c>
+      <c r="M31">
+        <v>-1.4</v>
+      </c>
+      <c r="N31">
+        <v>-1.7</v>
+      </c>
+      <c r="O31">
+        <v>-0.02700000000000002</v>
+      </c>
+      <c r="P31">
+        <v>-1.2</v>
+      </c>
+      <c r="Q31">
+        <v>-1</v>
+      </c>
+      <c r="R31">
+        <v>0.1000000000000001</v>
+      </c>
+      <c r="S31">
+        <v>-4.899999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>52</v>
+      </c>
+      <c r="D32" t="s">
+        <v>62</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+      <c r="F32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32">
+        <v>76</v>
+      </c>
+      <c r="I32">
+        <v>2468</v>
+      </c>
+      <c r="J32">
+        <v>7.5</v>
+      </c>
+      <c r="K32">
+        <v>20.2</v>
+      </c>
+      <c r="L32">
+        <v>0.371</v>
+      </c>
+      <c r="M32">
+        <v>5.1</v>
+      </c>
+      <c r="N32">
+        <v>6.6</v>
+      </c>
+      <c r="O32">
+        <v>0.779</v>
+      </c>
+      <c r="P32">
+        <v>4.8</v>
+      </c>
+      <c r="Q32">
+        <v>8.6</v>
+      </c>
+      <c r="R32">
+        <v>2.9</v>
+      </c>
+      <c r="S32">
+        <v>20.1</v>
+      </c>
+      <c r="T32" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" t="s">
+        <v>66</v>
+      </c>
+      <c r="G33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <v>337</v>
+      </c>
+      <c r="J33">
+        <v>5.3</v>
+      </c>
+      <c r="K33">
+        <v>15.7</v>
+      </c>
+      <c r="L33">
+        <v>0.34</v>
+      </c>
+      <c r="M33">
+        <v>7.2</v>
+      </c>
+      <c r="N33">
+        <v>9.4</v>
+      </c>
+      <c r="O33">
+        <v>0.761</v>
+      </c>
+      <c r="P33">
+        <v>4.6</v>
+      </c>
+      <c r="Q33">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="R33">
+        <v>3.5</v>
+      </c>
+      <c r="S33">
+        <v>17.8</v>
+      </c>
+      <c r="T33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="I34">
+        <v>-2131</v>
+      </c>
+      <c r="J34">
+        <v>-2.2</v>
+      </c>
+      <c r="K34">
+        <v>-4.5</v>
+      </c>
+      <c r="L34">
+        <v>-0.03099999999999997</v>
+      </c>
+      <c r="M34">
+        <v>2.100000000000001</v>
+      </c>
+      <c r="N34">
+        <v>2.800000000000001</v>
+      </c>
+      <c r="O34">
+        <v>-0.01800000000000002</v>
+      </c>
+      <c r="P34">
+        <v>-0.2000000000000002</v>
+      </c>
+      <c r="Q34">
+        <v>1.1</v>
+      </c>
+      <c r="R34">
+        <v>0.6000000000000001</v>
+      </c>
+      <c r="S34">
+        <v>-2.300000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G35">
+        <v>75</v>
+      </c>
+      <c r="I35">
+        <v>2114</v>
+      </c>
+      <c r="J35">
+        <v>7.9</v>
+      </c>
+      <c r="K35">
+        <v>20.1</v>
+      </c>
+      <c r="L35">
+        <v>0.391</v>
+      </c>
+      <c r="M35">
+        <v>4.3</v>
+      </c>
+      <c r="N35">
+        <v>5.7</v>
+      </c>
+      <c r="O35">
+        <v>0.754</v>
+      </c>
+      <c r="P35">
+        <v>4.4</v>
+      </c>
+      <c r="Q35">
+        <v>9.9</v>
+      </c>
+      <c r="R35">
+        <v>2.3</v>
+      </c>
+      <c r="S35">
+        <v>20</v>
+      </c>
+      <c r="T35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="s">
+        <v>65</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36">
+        <v>14</v>
+      </c>
+      <c r="I36">
+        <v>474</v>
+      </c>
+      <c r="J36">
+        <v>6.5</v>
+      </c>
+      <c r="K36">
+        <v>18.3</v>
+      </c>
+      <c r="L36">
+        <v>0.357</v>
+      </c>
+      <c r="M36">
+        <v>3.9</v>
+      </c>
+      <c r="N36">
+        <v>5.8</v>
+      </c>
+      <c r="O36">
+        <v>0.6840000000000001</v>
+      </c>
+      <c r="P36">
+        <v>4.9</v>
+      </c>
+      <c r="Q36">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="R36">
+        <v>3.3</v>
+      </c>
+      <c r="S36">
+        <v>17</v>
+      </c>
+      <c r="T36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="I37">
+        <v>-1640</v>
+      </c>
+      <c r="J37">
+        <v>-1.4</v>
+      </c>
+      <c r="K37">
+        <v>-1.800000000000001</v>
+      </c>
+      <c r="L37">
+        <v>-0.03400000000000003</v>
+      </c>
+      <c r="M37">
+        <v>-0.3999999999999999</v>
+      </c>
+      <c r="N37">
+        <v>0.09999999999999964</v>
+      </c>
+      <c r="O37">
+        <v>-0.06999999999999995</v>
+      </c>
+      <c r="P37">
+        <v>0.5</v>
+      </c>
+      <c r="Q37">
+        <v>-0.5999999999999996</v>
+      </c>
+      <c r="R37">
+        <v>1</v>
+      </c>
+      <c r="S37">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>65</v>
+      </c>
+      <c r="F38" t="s">
+        <v>66</v>
+      </c>
+      <c r="G38">
+        <v>76</v>
+      </c>
+      <c r="I38">
+        <v>1975</v>
+      </c>
+      <c r="J38">
+        <v>7.1</v>
+      </c>
+      <c r="K38">
+        <v>18</v>
+      </c>
+      <c r="L38">
+        <v>0.397</v>
+      </c>
+      <c r="M38">
+        <v>4</v>
+      </c>
+      <c r="N38">
+        <v>5.4</v>
+      </c>
+      <c r="O38">
+        <v>0.735</v>
+      </c>
+      <c r="P38">
+        <v>3.5</v>
+      </c>
+      <c r="Q38">
+        <v>9.4</v>
+      </c>
+      <c r="R38">
+        <v>3.2</v>
+      </c>
+      <c r="S38">
+        <v>18.3</v>
+      </c>
+      <c r="T38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" t="s">
+        <v>31</v>
+      </c>
+      <c r="C39" t="s">
+        <v>54</v>
+      </c>
+      <c r="D39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39">
+        <v>13</v>
+      </c>
+      <c r="I39">
+        <v>393</v>
+      </c>
+      <c r="J39">
+        <v>6.6</v>
+      </c>
+      <c r="K39">
+        <v>18.7</v>
+      </c>
+      <c r="L39">
+        <v>0.353</v>
+      </c>
+      <c r="M39">
+        <v>3.6</v>
+      </c>
+      <c r="N39">
+        <v>4.3</v>
+      </c>
+      <c r="O39">
+        <v>0.83</v>
+      </c>
+      <c r="P39">
+        <v>2.9</v>
+      </c>
+      <c r="Q39">
+        <v>10.6</v>
+      </c>
+      <c r="R39">
+        <v>4</v>
+      </c>
+      <c r="S39">
+        <v>16.8</v>
+      </c>
+      <c r="T39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="I40">
+        <v>-1582</v>
+      </c>
+      <c r="J40">
+        <v>-0.5</v>
+      </c>
+      <c r="K40">
+        <v>0.6999999999999993</v>
+      </c>
+      <c r="L40">
+        <v>-0.04400000000000004</v>
+      </c>
+      <c r="M40">
+        <v>-0.3999999999999999</v>
+      </c>
+      <c r="N40">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="O40">
+        <v>0.09499999999999997</v>
+      </c>
+      <c r="P40">
+        <v>-0.6000000000000001</v>
+      </c>
+      <c r="Q40">
+        <v>1.199999999999999</v>
+      </c>
+      <c r="R40">
+        <v>0.7999999999999998</v>
+      </c>
+      <c r="S40">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="I41">
+        <v>34</v>
+      </c>
+      <c r="J41">
+        <v>1.1</v>
+      </c>
+      <c r="K41">
+        <v>3.2</v>
+      </c>
+      <c r="L41">
+        <v>0.333</v>
+      </c>
+      <c r="M41">
+        <v>3.2</v>
+      </c>
+      <c r="N41">
+        <v>3.2</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+      <c r="P41">
+        <v>5.3</v>
+      </c>
+      <c r="Q41">
+        <v>10.6</v>
+      </c>
+      <c r="R41">
+        <v>11.6</v>
+      </c>
+      <c r="S41">
+        <v>5.3</v>
+      </c>
+      <c r="T41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" t="s">
+        <v>62</v>
+      </c>
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+      <c r="G43">
+        <v>917</v>
+      </c>
+      <c r="I43">
+        <v>30131</v>
+      </c>
+      <c r="J43">
+        <v>6.9</v>
+      </c>
+      <c r="K43">
+        <v>18.3</v>
+      </c>
+      <c r="L43">
+        <v>0.375</v>
+      </c>
+      <c r="M43">
+        <v>5.2</v>
+      </c>
+      <c r="N43">
+        <v>6.4</v>
+      </c>
+      <c r="O43">
+        <v>0.803</v>
+      </c>
+      <c r="P43">
+        <v>5.1</v>
+      </c>
+      <c r="Q43">
+        <v>7.9</v>
+      </c>
+      <c r="R43">
+        <v>2.4</v>
+      </c>
+      <c r="S43">
+        <v>19</v>
+      </c>
+      <c r="T43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" t="s">
+        <v>62</v>
+      </c>
+      <c r="E44" t="s">
+        <v>65</v>
+      </c>
+      <c r="G44">
+        <v>109</v>
+      </c>
+      <c r="I44">
+        <v>4120</v>
+      </c>
+      <c r="J44">
+        <v>5.9</v>
+      </c>
+      <c r="K44">
+        <v>17.2</v>
+      </c>
+      <c r="L44">
+        <v>0.342</v>
+      </c>
+      <c r="M44">
+        <v>5.5</v>
+      </c>
+      <c r="N44">
+        <v>6.9</v>
+      </c>
+      <c r="O44">
+        <v>0.801</v>
+      </c>
+      <c r="P44">
+        <v>4.6</v>
+      </c>
+      <c r="Q44">
+        <v>8.1</v>
+      </c>
+      <c r="R44">
+        <v>2.7</v>
+      </c>
+      <c r="S44">
+        <v>17.4</v>
+      </c>
+      <c r="T44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="I45">
+        <v>-26011</v>
+      </c>
+      <c r="J45">
+        <v>-1</v>
+      </c>
+      <c r="K45">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="L45">
+        <v>-0.03299999999999997</v>
+      </c>
+      <c r="M45">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="N45">
+        <v>0.5</v>
+      </c>
+      <c r="O45">
+        <v>-0.002000000000000002</v>
+      </c>
+      <c r="P45">
+        <v>-0.5</v>
+      </c>
+      <c r="Q45">
+        <v>0.1999999999999993</v>
+      </c>
+      <c r="R45">
+        <v>0.3000000000000003</v>
+      </c>
+      <c r="S45">
+        <v>-1.600000000000001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" t="s">
+        <v>64</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="I46">
+        <v>34</v>
+      </c>
+      <c r="J46">
+        <v>1.1</v>
+      </c>
+      <c r="K46">
+        <v>3.2</v>
+      </c>
+      <c r="L46">
+        <v>0.333</v>
+      </c>
+      <c r="M46">
+        <v>3.2</v>
+      </c>
+      <c r="N46">
+        <v>3.2</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+      <c r="P46">
+        <v>5.3</v>
+      </c>
+      <c r="Q46">
+        <v>10.6</v>
+      </c>
+      <c r="R46">
+        <v>11.6</v>
+      </c>
+      <c r="S46">
+        <v>5.3</v>
+      </c>
+      <c r="T46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E48" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48">
+        <v>924</v>
+      </c>
+      <c r="I48">
+        <v>30165</v>
+      </c>
+      <c r="J48">
+        <v>6.9</v>
+      </c>
+      <c r="K48">
+        <v>18.3</v>
+      </c>
+      <c r="L48">
+        <v>0.375</v>
+      </c>
+      <c r="M48">
+        <v>5.2</v>
+      </c>
+      <c r="N48">
+        <v>6.4</v>
+      </c>
+      <c r="O48">
+        <v>0.803</v>
+      </c>
+      <c r="P48">
+        <v>5.1</v>
+      </c>
+      <c r="Q48">
+        <v>7.9</v>
+      </c>
+      <c r="R48">
+        <v>2.5</v>
+      </c>
+      <c r="S48">
+        <v>19</v>
+      </c>
+      <c r="T48" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>41</v>
+      </c>
+      <c r="E49" t="s">
+        <v>65</v>
+      </c>
+      <c r="G49">
+        <v>109</v>
+      </c>
+      <c r="I49">
+        <v>4120</v>
+      </c>
+      <c r="J49">
+        <v>5.9</v>
+      </c>
+      <c r="K49">
+        <v>17.2</v>
+      </c>
+      <c r="L49">
+        <v>0.342</v>
+      </c>
+      <c r="M49">
+        <v>5.5</v>
+      </c>
+      <c r="N49">
+        <v>6.9</v>
+      </c>
+      <c r="O49">
+        <v>0.801</v>
+      </c>
+      <c r="P49">
+        <v>4.6</v>
+      </c>
+      <c r="Q49">
+        <v>8.1</v>
+      </c>
+      <c r="R49">
+        <v>2.7</v>
+      </c>
+      <c r="S49">
+        <v>17.4</v>
+      </c>
+      <c r="T49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="I50">
+        <v>-26045</v>
+      </c>
+      <c r="J50">
+        <v>-1</v>
+      </c>
+      <c r="K50">
+        <v>-1.100000000000001</v>
+      </c>
+      <c r="L50">
+        <v>-0.03299999999999997</v>
+      </c>
+      <c r="M50">
+        <v>0.2999999999999998</v>
+      </c>
+      <c r="N50">
+        <v>0.5</v>
+      </c>
+      <c r="O50">
+        <v>-0.002000000000000002</v>
+      </c>
+      <c r="P50">
+        <v>-0.5</v>
+      </c>
+      <c r="Q50">
+        <v>0.1999999999999993</v>
+      </c>
+      <c r="R50">
+        <v>0.2000000000000002</v>
+      </c>
+      <c r="S50">
+        <v>-1.600000000000001</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3423,10 +5834,10 @@
         <v>2</v>
       </c>
       <c r="J4">
-        <v>-0.1189999999999999</v>
+        <v>-0.119</v>
       </c>
       <c r="K4">
-        <v>-0.03499999999999998</v>
+        <v>-0.03500000000000003</v>
       </c>
       <c r="Q4">
         <v>-2.6</v>
@@ -3567,7 +5978,7 @@
         <v>-7</v>
       </c>
       <c r="T7">
-        <v>0.08899999999999997</v>
+        <v>0.089</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -3699,7 +6110,7 @@
         <v>-6.3</v>
       </c>
       <c r="T10">
-        <v>0.04900000000000002</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -3816,7 +6227,7 @@
         <v>-4.599999999999998</v>
       </c>
       <c r="J13">
-        <v>-0.04099999999999998</v>
+        <v>-0.04100000000000004</v>
       </c>
       <c r="K13">
         <v>0.233</v>
@@ -3963,7 +6374,7 @@
         <v>-7.399999999999999</v>
       </c>
       <c r="T16">
-        <v>-0.06699999999999998</v>
+        <v>-0.067</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -4227,7 +6638,7 @@
         <v>-7.600000000000001</v>
       </c>
       <c r="T22">
-        <v>-0.04400000000000001</v>
+        <v>-0.04399999999999998</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -4309,7 +6720,7 @@
         <v>17.6</v>
       </c>
       <c r="J24">
-        <v>0.4320000000000001</v>
+        <v>0.432</v>
       </c>
       <c r="K24">
         <v>0.383</v>
@@ -4344,10 +6755,10 @@
         <v>-0.2999999999999972</v>
       </c>
       <c r="J25">
-        <v>0.01700000000000007</v>
+        <v>0.01700000000000002</v>
       </c>
       <c r="K25">
-        <v>0.1249999999999999</v>
+        <v>0.125</v>
       </c>
       <c r="Q25">
         <v>-0.3</v>
@@ -4359,7 +6770,7 @@
         <v>-3.9</v>
       </c>
       <c r="T25">
-        <v>0.04000000000000001</v>
+        <v>0.03999999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -4476,7 +6887,7 @@
         <v>-3.799999999999997</v>
       </c>
       <c r="J28">
-        <v>-0.04599999999999999</v>
+        <v>-0.04600000000000004</v>
       </c>
       <c r="K28">
         <v>0.119</v>
@@ -4787,7 +7198,7 @@
         <v>18.3</v>
       </c>
       <c r="J35">
-        <v>0.4429999999999999</v>
+        <v>0.443</v>
       </c>
       <c r="K35">
         <v>0.282</v>
@@ -4872,7 +7283,7 @@
         <v>-2.800000000000001</v>
       </c>
       <c r="J37">
-        <v>-0.03499999999999998</v>
+        <v>-0.03500000000000003</v>
       </c>
       <c r="K37">
         <v>0.03300000000000003</v>
@@ -4887,7 +7298,7 @@
         <v>-5.5</v>
       </c>
       <c r="T37">
-        <v>-0.06100000000000001</v>
+        <v>-0.06099999999999998</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -5004,7 +7415,7 @@
         <v>-2.200000000000001</v>
       </c>
       <c r="J40">
-        <v>-0.04099999999999993</v>
+        <v>-0.04100000000000004</v>
       </c>
       <c r="K40">
         <v>-0.07199999999999998</v>

</xml_diff>

<commit_message>
created separate scraper folder
</commit_message>
<xml_diff>
--- a/output/cousybo01.xlsx
+++ b/output/cousybo01.xlsx
@@ -9,8 +9,7 @@
   <sheets>
     <sheet name="per_game" sheetId="1" r:id="rId1"/>
     <sheet name="per_minute" sheetId="2" r:id="rId2"/>
-    <sheet name="per_poss" sheetId="3" r:id="rId3"/>
-    <sheet name="advanced" sheetId="4" r:id="rId4"/>
+    <sheet name="advanced" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -5583,18 +5582,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:V50"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>